<commit_message>
added the updated sencha file v2
</commit_message>
<xml_diff>
--- a/W6 Project/KanenOS_FinalProject_Deliverables.xlsx
+++ b/W6 Project/KanenOS_FinalProject_Deliverables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="16275" windowHeight="7485" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Customers can add their favorite items to their cart and pay for them</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Update product</t>
+  </si>
+  <si>
+    <t>Product Comment Js</t>
   </si>
 </sst>
 </file>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:E42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,8 +761,9 @@
         <v>23</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
+      <c r="D11" s="1"/>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -771,152 +775,155 @@
         <v>25</v>
       </c>
       <c r="D12" s="1"/>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
-      <c r="B13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
+      <c r="B13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
+      <c r="B14" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="C18" s="5" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="1"/>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="C24" s="1" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>22</v>
@@ -924,97 +931,97 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="30" spans="1:5">
-      <c r="C30" s="1" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="10" t="s">
-        <v>7</v>
-      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="1"/>
-      <c r="B37" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11">
-        <v>1.25</v>
-      </c>
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1"/>
       <c r="B38" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="11">
@@ -1024,20 +1031,21 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
+      <c r="B39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11">
+        <v>1.25</v>
+      </c>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="B40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:5">
       <c r="B41" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -1047,13 +1055,23 @@
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="B43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add log4j file size config
</commit_message>
<xml_diff>
--- a/W6 Project/KanenOS_FinalProject_Deliverables.xlsx
+++ b/W6 Project/KanenOS_FinalProject_Deliverables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>Customers can add their favorite items to their cart and pay for them</t>
   </si>
@@ -105,9 +105,6 @@
     <t>DAOImpl</t>
   </si>
   <si>
-    <t>1 Manday</t>
-  </si>
-  <si>
     <t>UI Panel</t>
   </si>
   <si>
@@ -195,30 +192,29 @@
     <t>1 hr</t>
   </si>
   <si>
-    <t>fix some JPA issues</t>
-  </si>
-  <si>
     <t>Add Product UI</t>
   </si>
   <si>
     <t>Update product</t>
+  </si>
+  <si>
+    <t>fix JPA</t>
+  </si>
+  <si>
+    <t>resolved by Teacher Mike (5 mins)</t>
+  </si>
+  <si>
+    <t>ready for testing in UI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,17 +301,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -628,10 +623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:E42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,28 +634,28 @@
     <col min="1" max="1" width="78.42578125" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="3"/>
+      <c r="C2" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" s="4"/>
-      <c r="C2" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -679,23 +674,23 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -703,12 +698,12 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -716,12 +711,12 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -729,12 +724,12 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -742,7 +737,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -759,7 +754,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -774,17 +769,17 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -799,38 +794,38 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="C18" s="5" t="s">
-        <v>46</v>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -842,18 +837,20 @@
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>51</v>
+      <c r="B21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -863,11 +860,11 @@
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="C24" s="1" t="s">
@@ -881,7 +878,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>16</v>
@@ -892,22 +889,22 @@
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="1"/>
@@ -916,9 +913,9 @@
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="1"/>
@@ -935,53 +932,49 @@
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
+      <c r="B31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="C31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="10" t="s">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="1"/>
@@ -992,68 +985,88 @@
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1"/>
-      <c r="B37" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11">
+      <c r="B37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10">
         <v>1.25</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1"/>
-      <c r="B38" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11">
+      <c r="B38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10">
         <v>1.25</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="B40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
     </row>
     <row r="41" spans="1:5">
       <c r="B41" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="B43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added ppt, will add diagrams later
</commit_message>
<xml_diff>
--- a/W6 Project/KanenOS_FinalProject_Deliverables.xlsx
+++ b/W6 Project/KanenOS_FinalProject_Deliverables.xlsx
@@ -896,7 +896,7 @@
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -907,7 +907,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -920,7 +920,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -931,7 +931,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="5" t="s">

</xml_diff>